<commit_message>
update of parameter file templates with LATERAL IA classes
</commit_message>
<xml_diff>
--- a/param_file_templates/Excel/GROUND_fc_simple_salt_seb.xlsx
+++ b/param_file_templates/Excel/GROUND_fc_simple_salt_seb.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="159">
   <si>
     <t xml:space="preserve">    </t>
   </si>
@@ -59,9 +59,6 @@
     <t>surface emissivity</t>
   </si>
   <si>
-    <t>height of air temperature</t>
-  </si>
-  <si>
     <t>roughness length</t>
   </si>
   <si>
@@ -116,9 +113,6 @@
     <t>lower</t>
   </si>
   <si>
-    <t>geothermal heat flux</t>
-  </si>
-  <si>
     <t>TOP</t>
   </si>
   <si>
@@ -137,9 +131,6 @@
     <t>geographical coordinates</t>
   </si>
   <si>
-    <t>a.s.l.</t>
-  </si>
-  <si>
     <t>domain_depth</t>
   </si>
   <si>
@@ -200,9 +191,6 @@
     <t>STRAT_linear</t>
   </si>
   <si>
-    <t>should match a GRID point, model domain extends to this depth</t>
-  </si>
-  <si>
     <t>dt_max</t>
   </si>
   <si>
@@ -242,9 +230,6 @@
     <t>[y]</t>
   </si>
   <si>
-    <t>if left empty, the entire output will be written out at the end</t>
-  </si>
-  <si>
     <t>provide in format dd.mm.yyyy; if left empty, the last timestamp of the forcing data set will be used</t>
   </si>
   <si>
@@ -386,12 +371,6 @@
     <t>deltaT</t>
   </si>
   <si>
-    <t xml:space="preserve">area of the </t>
-  </si>
-  <si>
-    <t>OUT_all</t>
-  </si>
-  <si>
     <t>GROUND_fcSimple_salt_seb</t>
   </si>
   <si>
@@ -414,6 +393,114 @@
   </si>
   <si>
     <t>SUBSURFACE_CLASS</t>
+  </si>
+  <si>
+    <t>LAT_WATER_RESERVOIR</t>
+  </si>
+  <si>
+    <t>list of LATERAL INTERACTION classes to be used for the run, must be initialized below</t>
+  </si>
+  <si>
+    <t>OUT_all_lateral</t>
+  </si>
+  <si>
+    <t>timestep of output</t>
+  </si>
+  <si>
+    <t>date of the year at which the output is written to an output file</t>
+  </si>
+  <si>
+    <t>interval after which output file is written - if left empty, the entire output will be written out at the end</t>
+  </si>
+  <si>
+    <t>name of the file with forcing data</t>
+  </si>
+  <si>
+    <t>surface elevation a.s.l.</t>
+  </si>
+  <si>
+    <t>vertical extent of the model domain - should match a GRID point</t>
+  </si>
+  <si>
+    <t>area of the model realization</t>
+  </si>
+  <si>
+    <t>geothermal heat flux at lower boundary</t>
+  </si>
+  <si>
+    <t>height at which air temperature is provided</t>
+  </si>
+  <si>
+    <t>LATERAL_IA_CLASS</t>
+  </si>
+  <si>
+    <t>LAT_SEEPAGE_FACE_WATER</t>
+  </si>
+  <si>
+    <t>upperElevation</t>
+  </si>
+  <si>
+    <t>[m] a.s.l.</t>
+  </si>
+  <si>
+    <t>upper elevation of seepage face, set very high value instead of infinity</t>
+  </si>
+  <si>
+    <t>lowerElevation</t>
+  </si>
+  <si>
+    <t>lower elevation  of seepage face, set very low value instead of minus infinity</t>
+  </si>
+  <si>
+    <t>hardBottom_cutoff</t>
+  </si>
+  <si>
+    <t>threshold volumetric water content below which a grid cell is considered "hard", i.e. impermeable to water</t>
+  </si>
+  <si>
+    <t>distance_seepageFace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance to seepage face, needs to be adjusted to fit the area and geometry of the model realization  </t>
+  </si>
+  <si>
+    <t>seepage_contact_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lateral contact length of seepage face, needs to be adjusted to fit the area and geometry of the model realization  </t>
+  </si>
+  <si>
+    <t>reservoir_elevation</t>
+  </si>
+  <si>
+    <t>elevation of water reservoir</t>
+  </si>
+  <si>
+    <t>reservoir_temperature</t>
+  </si>
+  <si>
+    <t>water reservoir temperature  - if empty, water added at the temperature of the respective grid cell - only active for Xice classes</t>
+  </si>
+  <si>
+    <t>distance_reservoir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distance to water reservoir, needs to be adjusted to fit the area and geometry of the model realization  </t>
+  </si>
+  <si>
+    <t>reservoir_contact_length</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lateral contact length of water reservoir, needs to be adjusted to fit the area and geometry of the model realization  </t>
+  </si>
+  <si>
+    <t>LAT_REMOVE_SURFACE_WATER</t>
+  </si>
+  <si>
+    <t>NO_PARAMERTERS_REQUIRED</t>
+  </si>
+  <si>
+    <t>LAT_REMOVE_SUBSURFACE_WATER</t>
   </si>
 </sst>
 </file>
@@ -755,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F188"/>
+  <dimension ref="A1:F187"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
-      <selection activeCell="C136" sqref="C136"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="A148" sqref="A148"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,179 +858,181 @@
     <col min="7" max="7" width="15.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="B5" t="s">
         <v>86</v>
       </c>
-      <c r="B3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="D5" t="s">
         <v>87</v>
       </c>
-      <c r="B4" t="s">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="D4" t="s">
+      <c r="B6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="D6" t="s">
         <v>90</v>
       </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="D5" t="s">
+      <c r="B7" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="D7" t="s">
         <v>93</v>
       </c>
-      <c r="B6" t="s">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="D6" t="s">
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>97</v>
       </c>
-      <c r="D7" t="s">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
         <v>99</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
         <v>101</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
         <v>103</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10">
-        <v>1</v>
-      </c>
-      <c r="D10" t="s">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
         <v>105</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
+      <c r="B14" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="C14" t="s">
         <v>109</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13">
-        <v>1</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="E14" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B14" t="s">
-        <v>113</v>
-      </c>
-      <c r="C14" t="s">
-        <v>114</v>
-      </c>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>115</v>
       </c>
       <c r="B15">
         <v>0.25</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -954,23 +1043,23 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="B21" s="2">
         <v>1</v>
@@ -978,64 +1067,70 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B22">
         <v>0.25</v>
       </c>
       <c r="C22" t="s">
-        <v>68</v>
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>65</v>
+      </c>
+      <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="B23" t="s">
-        <v>69</v>
-      </c>
-      <c r="C23" t="s">
-        <v>70</v>
+      <c r="D23" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
         <v>67</v>
       </c>
-      <c r="B24">
-        <v>1</v>
-      </c>
-      <c r="C24" t="s">
-        <v>71</v>
-      </c>
       <c r="D24" t="s">
-        <v>72</v>
+        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C28" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2">
         <v>1</v>
@@ -1043,32 +1138,35 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>111</v>
+      </c>
+      <c r="D32" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B33" s="5"/>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D34" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -1077,12 +1175,12 @@
         <v>5</v>
       </c>
       <c r="D35" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B36">
         <v>1</v>
@@ -1091,37 +1189,37 @@
         <v>5</v>
       </c>
       <c r="D36" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B37">
         <v>70</v>
       </c>
       <c r="C37" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D37" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B38">
         <v>10</v>
       </c>
       <c r="C38" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B39">
         <v>20</v>
@@ -1130,12 +1228,12 @@
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>130</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40">
         <v>100</v>
@@ -1144,26 +1242,26 @@
         <v>6</v>
       </c>
       <c r="D40" t="s">
-        <v>58</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B41">
         <v>100</v>
       </c>
       <c r="C41" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D41" t="s">
-        <v>120</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B42">
         <v>0.05</v>
@@ -1172,12 +1270,12 @@
         <v>4</v>
       </c>
       <c r="D42" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B43">
         <v>2</v>
@@ -1186,30 +1284,30 @@
         <v>6</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>134</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B48" s="2">
         <v>1</v>
@@ -1217,13 +1315,13 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C50" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
@@ -1239,7 +1337,7 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1299,30 +1397,30 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B63" s="2">
         <v>1</v>
@@ -1330,257 +1428,257 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="C65" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E65" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F65" s="3" t="s">
-        <v>119</v>
+        <v>23</v>
+      </c>
+      <c r="B65" t="s">
+        <v>75</v>
+      </c>
+      <c r="C65" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>6</v>
       </c>
-      <c r="B66" t="s">
-        <v>5</v>
-      </c>
-      <c r="C66" t="s">
-        <v>5</v>
-      </c>
-      <c r="D66" t="s">
-        <v>5</v>
-      </c>
-      <c r="E66" t="s">
-        <v>123</v>
-      </c>
-      <c r="F66" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>0</v>
       </c>
-      <c r="B68">
-        <v>0.3</v>
+      <c r="B68" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="C68">
-        <v>0.5</v>
-      </c>
-      <c r="D68">
-        <v>0</v>
-      </c>
-      <c r="E68">
-        <v>500</v>
-      </c>
-      <c r="F68">
-        <v>-0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>0.5</v>
-      </c>
-      <c r="B69">
-        <v>0.5</v>
+        <v>10</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="C69">
-        <v>0.5</v>
-      </c>
-      <c r="D69">
-        <v>0</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>10</v>
-      </c>
-      <c r="B70">
-        <v>0.5</v>
-      </c>
-      <c r="C70">
-        <v>0.5</v>
-      </c>
-      <c r="D70">
-        <v>0</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
+      <c r="A70" t="s">
+        <v>30</v>
+      </c>
+      <c r="B70" s="4"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>32</v>
-      </c>
+      <c r="B71" s="4"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>41</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B72" s="4"/>
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>77</v>
+      </c>
+      <c r="B73" s="4"/>
+      <c r="C73" s="8"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
+      <c r="A74" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A76" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B77" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B78" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="2" t="s">
+      <c r="B80" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C80" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B75" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="B76" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+      <c r="D80" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>6</v>
+      </c>
+      <c r="B81" t="s">
+        <v>5</v>
+      </c>
+      <c r="C81" t="s">
+        <v>5</v>
+      </c>
+      <c r="D81" t="s">
+        <v>5</v>
+      </c>
+      <c r="E81" t="s">
+        <v>116</v>
+      </c>
+      <c r="F81" t="s">
         <v>24</v>
       </c>
-      <c r="B78" t="s">
-        <v>80</v>
-      </c>
-      <c r="C78" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A83">
         <v>0</v>
       </c>
-      <c r="B81" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82">
+      <c r="B83">
+        <v>0.3</v>
+      </c>
+      <c r="C83">
+        <v>0.5</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>500</v>
+      </c>
+      <c r="F83">
+        <v>-0.5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>0.5</v>
+      </c>
+      <c r="B84">
+        <v>0.5</v>
+      </c>
+      <c r="C84">
+        <v>0.5</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A85">
         <v>10</v>
       </c>
-      <c r="B82" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>32</v>
-      </c>
-      <c r="B83" s="4"/>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B84" s="4"/>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>83</v>
-      </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="8"/>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B85">
+        <v>0.5</v>
+      </c>
+      <c r="C85">
+        <v>0.5</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>82</v>
-      </c>
-      <c r="B86" s="4"/>
-      <c r="C86" s="8"/>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A90" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B91" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A93" s="3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C90" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B91" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="B93" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>6</v>
       </c>
       <c r="B94" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>0</v>
       </c>
@@ -1622,31 +1720,31 @@
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C107" s="6"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B108" s="7">
         <v>1</v>
@@ -1659,13 +1757,13 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B110" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C110" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C110" s="6" t="s">
+      <c r="D110" t="s">
         <v>17</v>
-      </c>
-      <c r="D110" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.25">
@@ -1716,12 +1814,12 @@
         <v>6</v>
       </c>
       <c r="E113" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B114">
         <v>100</v>
@@ -1730,15 +1828,15 @@
         <v>100</v>
       </c>
       <c r="D114" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E114" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="B115">
         <v>1.5</v>
@@ -1750,12 +1848,12 @@
         <v>5</v>
       </c>
       <c r="E115" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B116" s="6">
         <v>3600</v>
@@ -1767,12 +1865,12 @@
         <v>7</v>
       </c>
       <c r="E116" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B117" s="6">
         <v>50000</v>
@@ -1784,12 +1882,12 @@
         <v>8</v>
       </c>
       <c r="E117" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
@@ -1797,20 +1895,20 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B123" s="7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B124" s="7">
         <v>1</v>
@@ -1821,13 +1919,13 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B126" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C126" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C126" s="6" t="s">
+      <c r="D126" t="s">
         <v>17</v>
-      </c>
-      <c r="D126" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -1878,12 +1976,12 @@
         <v>6</v>
       </c>
       <c r="E129" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B130" s="6">
         <v>100</v>
@@ -1906,7 +2004,7 @@
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B132" s="6">
         <v>3600</v>
@@ -1918,12 +2016,12 @@
         <v>7</v>
       </c>
       <c r="E132" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B133" s="6">
         <v>50000</v>
@@ -1935,12 +2033,12 @@
         <v>8</v>
       </c>
       <c r="E133" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B134" s="6"/>
       <c r="C134" s="6"/>
@@ -1950,21 +2048,21 @@
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C138" s="6"/>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B139" s="6">
         <v>1</v>
@@ -1977,18 +2075,18 @@
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B141" t="s">
+        <v>15</v>
+      </c>
+      <c r="C141" t="s">
         <v>16</v>
       </c>
-      <c r="C141" t="s">
+      <c r="D141" t="s">
         <v>17</v>
-      </c>
-      <c r="D141" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="4" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B142">
         <v>0.25</v>
@@ -1997,7 +2095,7 @@
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B143" s="6"/>
       <c r="C143" s="6"/>
@@ -2006,172 +2104,342 @@
       <c r="A144" s="4"/>
       <c r="C144" s="6"/>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" s="1"/>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A146" s="2"/>
-      <c r="B146" s="7"/>
-      <c r="C146" s="6"/>
-    </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A147" s="2"/>
-      <c r="B147" s="7"/>
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A147" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B147" t="s">
+        <v>14</v>
+      </c>
       <c r="C147" s="6"/>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B148" s="6"/>
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A148" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="B148" s="6">
+        <v>1</v>
+      </c>
       <c r="C148" s="6"/>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B149" s="6"/>
       <c r="C149" s="6"/>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B150" s="6"/>
-      <c r="C150" s="6"/>
-    </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B151" s="6"/>
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>15</v>
+      </c>
+      <c r="C150" t="s">
+        <v>16</v>
+      </c>
+      <c r="D150" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>137</v>
+      </c>
+      <c r="B151" s="6">
+        <v>100000</v>
+      </c>
       <c r="C151" s="6"/>
-    </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B152" s="6"/>
+      <c r="D151" t="s">
+        <v>138</v>
+      </c>
+      <c r="E151" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A152" t="s">
+        <v>140</v>
+      </c>
+      <c r="B152" s="6">
+        <v>15</v>
+      </c>
       <c r="C152" s="6"/>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B153" s="6"/>
-      <c r="C153" s="6"/>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B154" s="6"/>
+      <c r="D152" t="s">
+        <v>138</v>
+      </c>
+      <c r="E152" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>142</v>
+      </c>
+      <c r="B153" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C153" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="D153" t="s">
+        <v>5</v>
+      </c>
+      <c r="E153" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A154" t="s">
+        <v>144</v>
+      </c>
+      <c r="B154" s="6">
+        <v>10</v>
+      </c>
       <c r="C154" s="6"/>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B155" s="6"/>
+      <c r="D154" t="s">
+        <v>6</v>
+      </c>
+      <c r="E154" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>146</v>
+      </c>
+      <c r="B155" s="6">
+        <v>10</v>
+      </c>
       <c r="C155" s="6"/>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D155" t="s">
+        <v>6</v>
+      </c>
+      <c r="E155" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A156" t="s">
+        <v>37</v>
+      </c>
       <c r="B156" s="6"/>
       <c r="C156" s="6"/>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B157" s="6"/>
       <c r="C157" s="6"/>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B158" s="6"/>
       <c r="C158" s="6"/>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B159" s="6"/>
-      <c r="C159" s="6"/>
-    </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B160" s="6"/>
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A159" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B160" t="s">
+        <v>14</v>
+      </c>
       <c r="C160" s="6"/>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B161" s="6"/>
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B161" s="6">
+        <v>1</v>
+      </c>
       <c r="C161" s="6"/>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B162" s="6"/>
       <c r="C162" s="6"/>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B163" s="6"/>
-      <c r="C163" s="6"/>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B164" s="6"/>
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B163" t="s">
+        <v>15</v>
+      </c>
+      <c r="C163" t="s">
+        <v>16</v>
+      </c>
+      <c r="D163" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A164" t="s">
+        <v>148</v>
+      </c>
+      <c r="B164" s="6">
+        <v>18</v>
+      </c>
       <c r="C164" s="6"/>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D164" t="s">
+        <v>138</v>
+      </c>
+      <c r="E164" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>150</v>
+      </c>
       <c r="B165" s="6"/>
       <c r="C165" s="6"/>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B166" s="6"/>
-      <c r="C166" s="6"/>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B167" s="6"/>
+      <c r="D165" t="s">
+        <v>24</v>
+      </c>
+      <c r="E165" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A166" t="s">
+        <v>142</v>
+      </c>
+      <c r="B166" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="C166" s="6">
+        <v>0.03</v>
+      </c>
+      <c r="D166" t="s">
+        <v>5</v>
+      </c>
+      <c r="E166" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>152</v>
+      </c>
+      <c r="B167" s="6">
+        <v>10</v>
+      </c>
       <c r="C167" s="6"/>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B170" s="6"/>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B171" s="6"/>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="1"/>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A173" s="2"/>
-      <c r="B173" s="7"/>
-      <c r="C173" s="6"/>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A174" s="2"/>
-      <c r="B174" s="7"/>
-      <c r="C174" s="6"/>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B175" s="6"/>
-      <c r="C175" s="6"/>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B176" s="6"/>
-      <c r="C176" s="6"/>
-    </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B177" s="6"/>
-      <c r="C177" s="6"/>
-    </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B178" s="6"/>
-      <c r="C178" s="6"/>
-    </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B179" s="6"/>
-      <c r="C179" s="6"/>
-    </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B180" s="6"/>
-      <c r="C180" s="6"/>
-    </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B181" s="6"/>
-      <c r="C181" s="6"/>
-    </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B182" s="6"/>
-      <c r="C182" s="6"/>
-    </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B183" s="6"/>
-      <c r="C183" s="6"/>
-    </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B184" s="6"/>
-      <c r="C184" s="6"/>
-    </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B185" s="6"/>
-      <c r="C185" s="6"/>
-    </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B186" s="6"/>
-      <c r="C186" s="6"/>
-    </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B187" s="6"/>
-      <c r="C187" s="6"/>
-    </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C188" s="6"/>
+      <c r="D167" t="s">
+        <v>6</v>
+      </c>
+      <c r="E167" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A168" t="s">
+        <v>154</v>
+      </c>
+      <c r="B168" s="6">
+        <v>10</v>
+      </c>
+      <c r="C168" s="6"/>
+      <c r="D168" t="s">
+        <v>6</v>
+      </c>
+      <c r="E168" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>37</v>
+      </c>
+      <c r="B169" s="6"/>
+      <c r="C169" s="6"/>
+    </row>
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B176" t="s">
+        <v>15</v>
+      </c>
+      <c r="C176" t="s">
+        <v>16</v>
+      </c>
+      <c r="D176" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A178" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A181" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B185" t="s">
+        <v>15</v>
+      </c>
+      <c r="C185" t="s">
+        <v>16</v>
+      </c>
+      <c r="D185" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A186" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>37</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>